<commit_message>
inverse from norm sent on second
</commit_message>
<xml_diff>
--- a/result/test1.xlsx
+++ b/result/test1.xlsx
@@ -423,16 +423,16 @@
         <v>4</v>
       </c>
       <c r="B2">
-        <v>0.9410582719356999</v>
+        <v>0.9646133682830931</v>
       </c>
       <c r="C2">
-        <v>0.9596994535519126</v>
+        <v>0.9496774193548387</v>
       </c>
       <c r="D2">
-        <v>0.9502874535001691</v>
+        <v>0.9570871261378414</v>
       </c>
       <c r="E2">
-        <v>1464</v>
+        <v>1550</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -440,16 +440,16 @@
         <v>5</v>
       </c>
       <c r="B3">
-        <v>0.9608493696084937</v>
+        <v>0.9470827679782904</v>
       </c>
       <c r="C3">
-        <v>0.9427083333333334</v>
+        <v>0.9627586206896551</v>
       </c>
       <c r="D3">
-        <v>0.9516924088070982</v>
+        <v>0.9548563611491109</v>
       </c>
       <c r="E3">
-        <v>1536</v>
+        <v>1450</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -457,16 +457,16 @@
         <v>6</v>
       </c>
       <c r="B4">
-        <v>0.951</v>
+        <v>0.956</v>
       </c>
       <c r="C4">
-        <v>0.951</v>
+        <v>0.956</v>
       </c>
       <c r="D4">
-        <v>0.951</v>
+        <v>0.956</v>
       </c>
       <c r="E4">
-        <v>0.951</v>
+        <v>0.956</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -474,13 +474,13 @@
         <v>7</v>
       </c>
       <c r="B5">
-        <v>0.9509538207720968</v>
+        <v>0.9558480681306918</v>
       </c>
       <c r="C5">
-        <v>0.951203893442623</v>
+        <v>0.956218020022247</v>
       </c>
       <c r="D5">
-        <v>0.9509899311536336</v>
+        <v>0.9559717436434761</v>
       </c>
       <c r="E5">
         <v>3000</v>
@@ -491,13 +491,13 @@
         <v>8</v>
       </c>
       <c r="B6">
-        <v>0.9511913139441703</v>
+        <v>0.9561402448024385</v>
       </c>
       <c r="C6">
-        <v>0.951</v>
+        <v>0.956</v>
       </c>
       <c r="D6">
-        <v>0.9510067906173169</v>
+        <v>0.956008923059955</v>
       </c>
       <c r="E6">
         <v>3000</v>

</xml_diff>